<commit_message>
modifiche al file con i tempi
</commit_message>
<xml_diff>
--- a/Dati.xlsx
+++ b/Dati.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo-my.sharepoint.com/personal/laura_cappelli6_studio_unibo_it/Documents/UNIBO/a.a. 2018-2019/ScalableAndCloudProgramming/ProgettoJAR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\IdeaProjects\Project-SCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{DF63CC63-3610-4A2B-A34C-7CE7B270DCBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{426CAB3F-4F27-4208-AA8B-4D637BFEFC6F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503FFDEF-FEFA-4211-AD53-FEB955B328DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{90149ABC-1584-4F15-AEC8-56C8B126FFFA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{90149ABC-1584-4F15-AEC8-56C8B126FFFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
   <si>
     <t>Citta</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Astar-locale</t>
   </si>
   <si>
-    <t>Astar</t>
-  </si>
-  <si>
     <t>BF-cloud</t>
   </si>
   <si>
@@ -61,6 +58,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Astar-Cloud</t>
+  </si>
+  <si>
+    <t>prova</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,50 +111,31 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9FFD9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="29">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -199,19 +183,346 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -219,25 +530,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD9FFD9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3348,7 +3702,7 @@
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -3378,13 +3732,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>355600</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
@@ -3750,33 +4104,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{273D63D3-33C7-4890-8705-800781828D44}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A2:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="11.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="4" width="11.6328125" customWidth="1"/>
     <col min="5" max="5" width="4.453125" style="4" customWidth="1"/>
-    <col min="6" max="9" width="11.6328125" customWidth="1"/>
+    <col min="6" max="13" width="10.7265625" customWidth="1"/>
+    <col min="14" max="18" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="F2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
+      <c r="F2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -3793,387 +4157,623 @@
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>7</v>
+      <c r="H3" s="14" t="s">
+        <v>6</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>98</v>
+      </c>
+      <c r="D4" s="8">
+        <v>282</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G4" s="10">
+        <v>33151</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="23">
+        <v>97024</v>
+      </c>
+      <c r="J4" s="27">
+        <v>95318</v>
+      </c>
+      <c r="K4" s="31">
+        <v>29277</v>
+      </c>
+      <c r="L4" s="31"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="39"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="13">
+        <v>2</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>192</v>
+      </c>
+      <c r="D5" s="8">
+        <v>592</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="10">
+        <v>72586</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="25">
+        <v>127275</v>
+      </c>
+      <c r="J5" s="28"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="20"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="13">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>290</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1060</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="10">
+        <v>101271</v>
+      </c>
+      <c r="H6" s="7"/>
+      <c r="I6" s="25">
+        <v>127078</v>
+      </c>
+      <c r="J6" s="28"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="20"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="13">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8">
+        <v>573</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2928</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="10">
+        <v>258570</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="25">
+        <v>467184</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="20"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="13">
+        <v>5</v>
+      </c>
+      <c r="B8" s="11">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8">
+        <v>748</v>
+      </c>
+      <c r="D8" s="8">
+        <v>4918</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="10">
+        <v>371508</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="20"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="13">
         <v>6</v>
       </c>
+      <c r="B9" s="11">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8">
+        <v>970</v>
+      </c>
+      <c r="D9" s="8">
+        <v>8238</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="20"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7">
-        <v>98</v>
-      </c>
-      <c r="D4" s="7">
-        <v>282</v>
-      </c>
-      <c r="F4">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="G4" s="7">
-        <v>33151</v>
-      </c>
-      <c r="I4" s="7">
-        <v>97024</v>
-      </c>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="13">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11">
+        <v>10</v>
+      </c>
+      <c r="C10" s="8">
+        <v>2243</v>
+      </c>
+      <c r="D10" s="8">
+        <v>34134</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="7"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="20"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="13">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11">
+        <v>15</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3671</v>
+      </c>
+      <c r="D11" s="8">
+        <v>77480</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="20"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="13">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11">
+        <v>20</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4945</v>
+      </c>
+      <c r="D12" s="8">
+        <v>127168</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="7">
         <v>2</v>
       </c>
-      <c r="B5">
-        <v>1.5</v>
-      </c>
-      <c r="C5" s="7">
-        <v>192</v>
-      </c>
-      <c r="D5" s="7">
-        <v>592</v>
-      </c>
-      <c r="G5" s="7">
-        <v>72586</v>
-      </c>
-      <c r="I5" s="7">
-        <v>127275</v>
-      </c>
+      <c r="G12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="20"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="11">
+        <v>25</v>
+      </c>
+      <c r="C13" s="8">
+        <v>6267</v>
+      </c>
+      <c r="D13" s="8">
+        <v>191406</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="7"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="20"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="13">
+        <v>11</v>
+      </c>
+      <c r="B14" s="11">
+        <v>35</v>
+      </c>
+      <c r="C14" s="8">
+        <v>9328</v>
+      </c>
+      <c r="D14" s="8">
+        <v>413286</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="20"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="13">
+        <v>12</v>
+      </c>
+      <c r="B15" s="11">
+        <v>40</v>
+      </c>
+      <c r="C15" s="8">
+        <v>10784</v>
+      </c>
+      <c r="D15" s="8">
+        <v>542218</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="20"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="13">
+        <v>13</v>
+      </c>
+      <c r="B16" s="11">
+        <v>50</v>
+      </c>
+      <c r="C16" s="8">
+        <v>13580</v>
+      </c>
+      <c r="D16" s="8">
+        <v>860506</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="7">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7">
-        <v>290</v>
-      </c>
-      <c r="D6" s="7">
-        <v>1060</v>
-      </c>
-      <c r="G6" s="7">
-        <v>101271</v>
-      </c>
-      <c r="I6" s="7"/>
+      <c r="G16" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="20"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7">
-        <v>573</v>
-      </c>
-      <c r="D7" s="7">
-        <v>2928</v>
-      </c>
-      <c r="G7" s="7">
-        <v>258570</v>
-      </c>
-      <c r="I7" s="7"/>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="13">
+        <v>14</v>
+      </c>
+      <c r="B17" s="11">
+        <v>55</v>
+      </c>
+      <c r="C17" s="8">
+        <v>14947</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1030150</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="7">
+        <v>3.3</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="20"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8" s="7">
-        <v>748</v>
-      </c>
-      <c r="D8" s="7">
-        <v>4918</v>
-      </c>
-      <c r="G8" s="7">
-        <v>371508</v>
-      </c>
-      <c r="I8" s="7"/>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="13">
+        <v>15</v>
+      </c>
+      <c r="B18" s="11">
+        <v>60</v>
+      </c>
+      <c r="C18" s="8">
+        <v>16309</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1217380</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="7">
+        <v>3.1</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7">
-        <v>970</v>
-      </c>
-      <c r="D9" s="7">
-        <v>8238</v>
-      </c>
-      <c r="F9">
-        <v>1.2</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="7"/>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="13">
+        <v>16</v>
+      </c>
+      <c r="B19" s="11">
+        <v>65</v>
+      </c>
+      <c r="C19" s="8">
+        <v>17706</v>
+      </c>
+      <c r="D19" s="8">
+        <v>1448340</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="20"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10" s="7">
-        <v>2243</v>
-      </c>
-      <c r="D10" s="7">
-        <v>34134</v>
-      </c>
-      <c r="F10">
-        <v>1.4</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="7"/>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="13">
+        <v>17</v>
+      </c>
+      <c r="B20" s="11">
+        <v>75</v>
+      </c>
+      <c r="C20" s="8">
+        <v>20389</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1914202</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="20"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="13">
+        <v>18</v>
+      </c>
+      <c r="B21" s="11">
+        <v>100</v>
+      </c>
+      <c r="C21" s="8">
+        <v>27272</v>
+      </c>
+      <c r="D21" s="8">
+        <v>3381342</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>15</v>
-      </c>
-      <c r="C11" s="7">
-        <v>3671</v>
-      </c>
-      <c r="D11" s="7">
-        <v>77480</v>
-      </c>
-      <c r="F11">
-        <v>1.8</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>20</v>
-      </c>
-      <c r="C12" s="7">
-        <v>4945</v>
-      </c>
-      <c r="D12" s="7">
-        <v>127168</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>25</v>
-      </c>
-      <c r="C13" s="7">
-        <v>6267</v>
-      </c>
-      <c r="D13" s="7">
-        <v>191406</v>
-      </c>
-      <c r="F13">
-        <v>2.1</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <v>35</v>
-      </c>
-      <c r="C14" s="7">
-        <v>9328</v>
-      </c>
-      <c r="D14" s="7">
-        <v>413286</v>
-      </c>
-      <c r="F14">
-        <v>2.5</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15">
-        <v>40</v>
-      </c>
-      <c r="C15" s="7">
-        <v>10784</v>
-      </c>
-      <c r="D15" s="7">
-        <v>542218</v>
-      </c>
-      <c r="F15">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16">
-        <v>50</v>
-      </c>
-      <c r="C16" s="7">
-        <v>13580</v>
-      </c>
-      <c r="D16" s="7">
-        <v>860506</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17">
-        <v>55</v>
-      </c>
-      <c r="C17" s="7">
-        <v>14947</v>
-      </c>
-      <c r="D17" s="7">
-        <v>1030150</v>
-      </c>
-      <c r="F17">
-        <v>3.3</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>15</v>
-      </c>
-      <c r="B18">
-        <v>60</v>
-      </c>
-      <c r="C18" s="7">
-        <v>16309</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1217380</v>
-      </c>
-      <c r="F18">
-        <v>3.1</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>16</v>
-      </c>
-      <c r="B19">
-        <v>65</v>
-      </c>
-      <c r="C19" s="7">
-        <v>17706</v>
-      </c>
-      <c r="D19" s="7">
-        <v>1448340</v>
-      </c>
-      <c r="F19">
-        <v>3.6</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>17</v>
-      </c>
-      <c r="B20">
-        <v>75</v>
-      </c>
-      <c r="C20" s="7">
-        <v>20389</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1914202</v>
-      </c>
-      <c r="F20">
-        <v>3.6</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>18</v>
-      </c>
-      <c r="B21">
-        <v>100</v>
-      </c>
-      <c r="C21" s="7">
-        <v>27272</v>
-      </c>
-      <c r="D21" s="7">
-        <v>3381342</v>
-      </c>
-      <c r="F21">
-        <v>5.9</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F2:J2"/>
+    <mergeCell ref="F2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>